<commit_message>
Fixed importing shopItems with Pokeball nbtTags
</commit_message>
<xml_diff>
--- a/Pixelmon Custom NPC Shop/Custom Items - 1.16.5.xlsx
+++ b/Pixelmon Custom NPC Shop/Custom Items - 1.16.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\PixelmonCustomization\Pixelmon Custom NPC Shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813659A5-E8FA-4728-99CB-93650E306455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CD6131-28D9-4C7A-B07B-700D61DFF11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="1231">
   <si>
     <t>Item Name</t>
   </si>
@@ -3637,6 +3637,96 @@
   </si>
   <si>
     <t>Relic Copper</t>
+  </si>
+  <si>
+    <t>Cherish Ball</t>
+  </si>
+  <si>
+    <t>Safari Ball</t>
+  </si>
+  <si>
+    <t>pixelmon:cherish_ball</t>
+  </si>
+  <si>
+    <t>pixelmon:safari_ball</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "dive_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "dusk_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "fast_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "friend_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "great_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "gs_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "heal_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "heavy_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "level_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "love_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "lure_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "luxury_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "master_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "moon_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "nest_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "net_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "park_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "poke_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "premier_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "quick_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "repeat_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "sport_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "timer_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "ultra_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "cherish_ball"}</t>
+  </si>
+  <si>
+    <t>{"PokeBallID": "safari_ball"}</t>
   </si>
 </sst>
 </file>
@@ -3963,11 +4053,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H539"/>
+  <dimension ref="A1:H541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A360" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I378" sqref="I378"/>
+      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G492" sqref="G492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,7 +4067,7 @@
     <col min="3" max="3" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -4154,7 +4244,6 @@
         <v>0</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -4170,7 +4259,6 @@
         <v>0</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -4186,7 +4274,6 @@
         <v>0</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -4202,7 +4289,6 @@
         <v>0</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -4218,7 +4304,6 @@
         <v>0</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -4234,7 +4319,6 @@
         <v>0</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -4250,7 +4334,6 @@
         <v>0</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -8781,7 +8864,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>798</v>
       </c>
@@ -8795,7 +8878,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>798</v>
       </c>
@@ -8809,7 +8892,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>798</v>
       </c>
@@ -8823,7 +8906,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>798</v>
       </c>
@@ -8837,7 +8920,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>798</v>
       </c>
@@ -8851,7 +8934,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>798</v>
       </c>
@@ -8865,7 +8948,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>798</v>
       </c>
@@ -8879,7 +8962,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>798</v>
       </c>
@@ -8893,7 +8976,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>798</v>
       </c>
@@ -8907,7 +8990,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>798</v>
       </c>
@@ -8921,7 +9004,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>798</v>
       </c>
@@ -8935,7 +9018,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>798</v>
       </c>
@@ -8949,7 +9032,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>798</v>
       </c>
@@ -8963,7 +9046,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>798</v>
       </c>
@@ -8977,7 +9060,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>798</v>
       </c>
@@ -8991,7 +9074,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>269</v>
       </c>
@@ -8999,13 +9082,19 @@
         <v>1165</v>
       </c>
       <c r="C352" t="s">
-        <v>1137</v>
+        <v>1124</v>
       </c>
       <c r="F352" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G352" t="s">
+        <v>1137</v>
+      </c>
+      <c r="H352" s="3" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>269</v>
       </c>
@@ -9013,13 +9102,19 @@
         <v>1166</v>
       </c>
       <c r="C353" t="s">
-        <v>1140</v>
+        <v>1124</v>
       </c>
       <c r="F353" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G353" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H353" s="3" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>269</v>
       </c>
@@ -9027,13 +9122,19 @@
         <v>1167</v>
       </c>
       <c r="C354" t="s">
-        <v>1132</v>
+        <v>1124</v>
       </c>
       <c r="F354" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G354" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H354" s="3" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>269</v>
       </c>
@@ -9041,13 +9142,19 @@
         <v>1168</v>
       </c>
       <c r="C355" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="F355" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G355" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H355" s="3" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>269</v>
       </c>
@@ -9055,13 +9162,19 @@
         <v>1169</v>
       </c>
       <c r="C356" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="F356" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G356" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H356" s="3" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>269</v>
       </c>
@@ -9069,7 +9182,7 @@
         <v>1170</v>
       </c>
       <c r="C357" t="s">
-        <v>1067</v>
+        <v>1124</v>
       </c>
       <c r="E357" s="1">
         <v>250000</v>
@@ -9077,8 +9190,14 @@
       <c r="F357" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G357" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H357" s="3" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>269</v>
       </c>
@@ -9086,13 +9205,19 @@
         <v>1171</v>
       </c>
       <c r="C358" t="s">
-        <v>1139</v>
+        <v>1124</v>
       </c>
       <c r="F358" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G358" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H358" s="3" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>269</v>
       </c>
@@ -9100,13 +9225,19 @@
         <v>1172</v>
       </c>
       <c r="C359" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="F359" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G359" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H359" s="3" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>269</v>
       </c>
@@ -9114,13 +9245,19 @@
         <v>1173</v>
       </c>
       <c r="C360" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="F360" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G360" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H360" s="3" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>269</v>
       </c>
@@ -9128,13 +9265,19 @@
         <v>1174</v>
       </c>
       <c r="C361" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="F361" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G361" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H361" s="3" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>269</v>
       </c>
@@ -9142,13 +9285,19 @@
         <v>1175</v>
       </c>
       <c r="C362" t="s">
-        <v>1142</v>
+        <v>1124</v>
       </c>
       <c r="F362" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G362" t="s">
+        <v>1142</v>
+      </c>
+      <c r="H362" s="3" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>269</v>
       </c>
@@ -9156,13 +9305,19 @@
         <v>1176</v>
       </c>
       <c r="C363" t="s">
-        <v>1138</v>
+        <v>1124</v>
       </c>
       <c r="F363" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G363" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H363" s="3" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>269</v>
       </c>
@@ -9170,7 +9325,7 @@
         <v>1</v>
       </c>
       <c r="C364" t="s">
-        <v>2</v>
+        <v>1124</v>
       </c>
       <c r="E364" s="1">
         <v>500000</v>
@@ -9178,8 +9333,14 @@
       <c r="F364" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G364" t="s">
+        <v>2</v>
+      </c>
+      <c r="H364" s="3" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>269</v>
       </c>
@@ -9187,13 +9348,19 @@
         <v>1177</v>
       </c>
       <c r="C365" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="F365" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G365" t="s">
+        <v>1128</v>
+      </c>
+      <c r="H365" s="3" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>269</v>
       </c>
@@ -9201,13 +9368,19 @@
         <v>1178</v>
       </c>
       <c r="C366" t="s">
-        <v>1135</v>
+        <v>1124</v>
       </c>
       <c r="F366" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G366" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H366" s="3" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>269</v>
       </c>
@@ -9215,13 +9388,19 @@
         <v>1179</v>
       </c>
       <c r="C367" t="s">
-        <v>1136</v>
+        <v>1124</v>
       </c>
       <c r="F367" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G367" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H367" s="3" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>269</v>
       </c>
@@ -9229,7 +9408,7 @@
         <v>1065</v>
       </c>
       <c r="C368" t="s">
-        <v>1066</v>
+        <v>1124</v>
       </c>
       <c r="E368" s="1">
         <v>500000</v>
@@ -9237,8 +9416,14 @@
       <c r="F368" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G368" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H368" s="3" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>269</v>
       </c>
@@ -9251,8 +9436,14 @@
       <c r="F369" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G369" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H369" s="3" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>269</v>
       </c>
@@ -9260,7 +9451,7 @@
         <v>370</v>
       </c>
       <c r="C370" t="s">
-        <v>143</v>
+        <v>1124</v>
       </c>
       <c r="E370" s="1">
         <v>200</v>
@@ -9268,8 +9459,14 @@
       <c r="F370" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G370" t="s">
+        <v>143</v>
+      </c>
+      <c r="H370" s="3" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>269</v>
       </c>
@@ -9277,13 +9474,19 @@
         <v>1181</v>
       </c>
       <c r="C371" t="s">
-        <v>1141</v>
+        <v>1124</v>
       </c>
       <c r="F371" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G371" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H371" s="3" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>269</v>
       </c>
@@ -9291,13 +9494,19 @@
         <v>1182</v>
       </c>
       <c r="C372" t="s">
-        <v>1133</v>
+        <v>1124</v>
       </c>
       <c r="F372" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G372" t="s">
+        <v>1133</v>
+      </c>
+      <c r="H372" s="3" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>269</v>
       </c>
@@ -9305,13 +9514,19 @@
         <v>1183</v>
       </c>
       <c r="C373" t="s">
-        <v>1143</v>
+        <v>1124</v>
       </c>
       <c r="F373" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G373" t="s">
+        <v>1143</v>
+      </c>
+      <c r="H373" s="3" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>269</v>
       </c>
@@ -9319,13 +9534,19 @@
         <v>1184</v>
       </c>
       <c r="C374" t="s">
-        <v>1134</v>
+        <v>1124</v>
       </c>
       <c r="F374" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G374" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H374" s="3" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>269</v>
       </c>
@@ -9333,136 +9554,154 @@
         <v>1185</v>
       </c>
       <c r="C375" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F375" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G375" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H375" s="3" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>1186</v>
+        <v>269</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C376" s="2" t="s">
-        <v>1189</v>
+        <v>1201</v>
+      </c>
+      <c r="C376" t="s">
+        <v>1124</v>
       </c>
       <c r="F376" s="1">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G376" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H376" s="3" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>1186</v>
+        <v>269</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>1200</v>
-      </c>
-      <c r="C377" s="2" t="s">
-        <v>1193</v>
+        <v>1202</v>
+      </c>
+      <c r="C377" t="s">
+        <v>1124</v>
       </c>
       <c r="F377" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G377" t="s">
+        <v>1204</v>
+      </c>
+      <c r="H377" s="3" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>1186</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>1194</v>
+        <v>1196</v>
       </c>
       <c r="C378" s="2" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="F378" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>1186</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
       <c r="C379" s="2" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="F379" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>1186</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>1199</v>
+        <v>1194</v>
       </c>
       <c r="C380" s="2" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="F380" s="1">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>1186</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="C381" s="2" t="s">
-        <v>1188</v>
+        <v>1191</v>
       </c>
       <c r="F381" s="1">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>1186</v>
       </c>
       <c r="B382" s="2" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F382" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A383" s="2" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F383" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A384" s="2" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B384" s="2" t="s">
         <v>1197</v>
       </c>
-      <c r="C382" s="2" t="s">
+      <c r="C384" s="2" t="s">
         <v>1190</v>
       </c>
-      <c r="F382" s="1">
+      <c r="F384" s="1">
         <v>10000</v>
-      </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A383" s="2" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B383" s="2" t="s">
-        <v>783</v>
-      </c>
-      <c r="C383" s="2" t="s">
-        <v>677</v>
-      </c>
-      <c r="E383" s="1">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A384" s="2" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B384" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="C384" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="E384" s="1">
-        <v>980</v>
       </c>
     </row>
     <row r="385" spans="1:8" x14ac:dyDescent="0.25">
@@ -9470,10 +9709,10 @@
         <v>1058</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="C385" s="2" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="E385" s="1">
         <v>980</v>
@@ -9484,10 +9723,10 @@
         <v>1058</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C386" s="2" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="E386" s="1">
         <v>980</v>
@@ -9498,10 +9737,10 @@
         <v>1058</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C387" s="2" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E387" s="1">
         <v>980</v>
@@ -9512,10 +9751,10 @@
         <v>1058</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C388" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E388" s="1">
         <v>980</v>
@@ -9526,10 +9765,10 @@
         <v>1058</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="E389" s="1">
         <v>980</v>
@@ -9537,42 +9776,30 @@
     </row>
     <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>776</v>
+        <v>1058</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>679</v>
+        <v>781</v>
       </c>
       <c r="C390" s="2" t="s">
-        <v>472</v>
+        <v>675</v>
       </c>
       <c r="E390" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G390" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="H390" s="3" t="s">
-        <v>474</v>
+        <v>980</v>
       </c>
     </row>
     <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>776</v>
+        <v>1058</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>688</v>
+        <v>784</v>
       </c>
       <c r="C391" s="2" t="s">
-        <v>472</v>
+        <v>678</v>
       </c>
       <c r="E391" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G391" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="H391" s="3" t="s">
-        <v>494</v>
+        <v>980</v>
       </c>
     </row>
     <row r="392" spans="1:8" x14ac:dyDescent="0.25">
@@ -9580,7 +9807,7 @@
         <v>776</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>472</v>
@@ -9589,10 +9816,10 @@
         <v>10000</v>
       </c>
       <c r="G392" s="3" t="s">
-        <v>495</v>
+        <v>473</v>
       </c>
       <c r="H392" s="3" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
     </row>
     <row r="393" spans="1:8" x14ac:dyDescent="0.25">
@@ -9600,7 +9827,7 @@
         <v>776</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>472</v>
@@ -9609,10 +9836,10 @@
         <v>10000</v>
       </c>
       <c r="G393" s="3" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="H393" s="3" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="394" spans="1:8" x14ac:dyDescent="0.25">
@@ -9620,7 +9847,7 @@
         <v>776</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>472</v>
@@ -9629,10 +9856,10 @@
         <v>10000</v>
       </c>
       <c r="G394" s="3" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="H394" s="3" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="395" spans="1:8" x14ac:dyDescent="0.25">
@@ -9640,7 +9867,7 @@
         <v>776</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>458</v>
+        <v>690</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>472</v>
@@ -9649,10 +9876,10 @@
         <v>10000</v>
       </c>
       <c r="G395" s="3" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="H395" s="3" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="396" spans="1:8" x14ac:dyDescent="0.25">
@@ -9660,7 +9887,7 @@
         <v>776</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>472</v>
@@ -9669,10 +9896,10 @@
         <v>10000</v>
       </c>
       <c r="G396" s="3" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H396" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.25">
@@ -9680,7 +9907,7 @@
         <v>776</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>70</v>
+        <v>458</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>472</v>
@@ -9689,10 +9916,10 @@
         <v>10000</v>
       </c>
       <c r="G397" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="H397" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="398" spans="1:8" x14ac:dyDescent="0.25">
@@ -9700,7 +9927,7 @@
         <v>776</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>472</v>
@@ -9709,10 +9936,10 @@
         <v>10000</v>
       </c>
       <c r="G398" s="3" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="H398" s="3" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="399" spans="1:8" x14ac:dyDescent="0.25">
@@ -9720,7 +9947,7 @@
         <v>776</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>694</v>
+        <v>70</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>472</v>
@@ -9729,10 +9956,10 @@
         <v>10000</v>
       </c>
       <c r="G399" s="3" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="H399" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.25">
@@ -9740,7 +9967,7 @@
         <v>776</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>472</v>
@@ -9749,10 +9976,10 @@
         <v>10000</v>
       </c>
       <c r="G400" s="3" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="H400" s="3" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.25">
@@ -9760,7 +9987,7 @@
         <v>776</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>680</v>
+        <v>694</v>
       </c>
       <c r="C401" s="2" t="s">
         <v>472</v>
@@ -9769,10 +9996,10 @@
         <v>10000</v>
       </c>
       <c r="G401" s="3" t="s">
-        <v>475</v>
+        <v>509</v>
       </c>
       <c r="H401" s="3" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
     </row>
     <row r="402" spans="1:8" x14ac:dyDescent="0.25">
@@ -9780,7 +10007,7 @@
         <v>776</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>472</v>
@@ -9789,10 +10016,10 @@
         <v>10000</v>
       </c>
       <c r="G402" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H402" s="3" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.25">
@@ -9800,7 +10027,7 @@
         <v>776</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>697</v>
+        <v>680</v>
       </c>
       <c r="C403" s="2" t="s">
         <v>472</v>
@@ -9809,10 +10036,10 @@
         <v>10000</v>
       </c>
       <c r="G403" s="3" t="s">
-        <v>515</v>
+        <v>475</v>
       </c>
       <c r="H403" s="3" t="s">
-        <v>516</v>
+        <v>476</v>
       </c>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.25">
@@ -9820,7 +10047,7 @@
         <v>776</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>472</v>
@@ -9829,10 +10056,10 @@
         <v>10000</v>
       </c>
       <c r="G404" s="3" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="H404" s="3" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.25">
@@ -9840,7 +10067,7 @@
         <v>776</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>472</v>
@@ -9849,10 +10076,10 @@
         <v>10000</v>
       </c>
       <c r="G405" s="3" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="H405" s="3" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="406" spans="1:8" x14ac:dyDescent="0.25">
@@ -9860,7 +10087,7 @@
         <v>776</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>472</v>
@@ -9869,10 +10096,10 @@
         <v>10000</v>
       </c>
       <c r="G406" s="3" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="H406" s="3" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="407" spans="1:8" x14ac:dyDescent="0.25">
@@ -9880,7 +10107,7 @@
         <v>776</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>472</v>
@@ -9889,10 +10116,10 @@
         <v>10000</v>
       </c>
       <c r="G407" s="3" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="H407" s="3" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="408" spans="1:8" x14ac:dyDescent="0.25">
@@ -9900,7 +10127,7 @@
         <v>776</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>472</v>
@@ -9909,10 +10136,10 @@
         <v>10000</v>
       </c>
       <c r="G408" s="3" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="H408" s="3" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="409" spans="1:8" x14ac:dyDescent="0.25">
@@ -9920,7 +10147,7 @@
         <v>776</v>
       </c>
       <c r="B409" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>472</v>
@@ -9929,10 +10156,10 @@
         <v>10000</v>
       </c>
       <c r="G409" s="3" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="H409" s="3" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="410" spans="1:8" x14ac:dyDescent="0.25">
@@ -9940,7 +10167,7 @@
         <v>776</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>472</v>
@@ -9949,10 +10176,10 @@
         <v>10000</v>
       </c>
       <c r="G410" s="3" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="H410" s="3" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="411" spans="1:8" x14ac:dyDescent="0.25">
@@ -9960,7 +10187,7 @@
         <v>776</v>
       </c>
       <c r="B411" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>472</v>
@@ -9969,10 +10196,10 @@
         <v>10000</v>
       </c>
       <c r="G411" s="3" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="H411" s="3" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="412" spans="1:8" x14ac:dyDescent="0.25">
@@ -9980,7 +10207,7 @@
         <v>776</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>681</v>
+        <v>704</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>472</v>
@@ -9989,10 +10216,10 @@
         <v>10000</v>
       </c>
       <c r="G412" s="3" t="s">
-        <v>477</v>
+        <v>529</v>
       </c>
       <c r="H412" s="3" t="s">
-        <v>478</v>
+        <v>530</v>
       </c>
     </row>
     <row r="413" spans="1:8" x14ac:dyDescent="0.25">
@@ -10000,7 +10227,7 @@
         <v>776</v>
       </c>
       <c r="B413" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>472</v>
@@ -10009,10 +10236,10 @@
         <v>10000</v>
       </c>
       <c r="G413" s="3" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H413" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.25">
@@ -10020,7 +10247,7 @@
         <v>776</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>707</v>
+        <v>681</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>472</v>
@@ -10029,10 +10256,10 @@
         <v>10000</v>
       </c>
       <c r="G414" s="3" t="s">
-        <v>535</v>
+        <v>477</v>
       </c>
       <c r="H414" s="3" t="s">
-        <v>536</v>
+        <v>478</v>
       </c>
     </row>
     <row r="415" spans="1:8" x14ac:dyDescent="0.25">
@@ -10040,7 +10267,7 @@
         <v>776</v>
       </c>
       <c r="B415" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>472</v>
@@ -10049,10 +10276,10 @@
         <v>10000</v>
       </c>
       <c r="G415" s="3" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="H415" s="3" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="416" spans="1:8" x14ac:dyDescent="0.25">
@@ -10060,7 +10287,7 @@
         <v>776</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>472</v>
@@ -10069,10 +10296,10 @@
         <v>10000</v>
       </c>
       <c r="G416" s="3" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="H416" s="3" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="417" spans="1:8" x14ac:dyDescent="0.25">
@@ -10080,7 +10307,7 @@
         <v>776</v>
       </c>
       <c r="B417" s="2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>472</v>
@@ -10089,10 +10316,10 @@
         <v>10000</v>
       </c>
       <c r="G417" s="3" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="H417" s="3" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="418" spans="1:8" x14ac:dyDescent="0.25">
@@ -10100,7 +10327,7 @@
         <v>776</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>472</v>
@@ -10109,10 +10336,10 @@
         <v>10000</v>
       </c>
       <c r="G418" s="3" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="H418" s="3" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.25">
@@ -10120,7 +10347,7 @@
         <v>776</v>
       </c>
       <c r="B419" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>472</v>
@@ -10129,10 +10356,10 @@
         <v>10000</v>
       </c>
       <c r="G419" s="3" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="H419" s="3" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="420" spans="1:8" x14ac:dyDescent="0.25">
@@ -10140,7 +10367,7 @@
         <v>776</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>472</v>
@@ -10149,10 +10376,10 @@
         <v>10000</v>
       </c>
       <c r="G420" s="3" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="H420" s="3" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="421" spans="1:8" x14ac:dyDescent="0.25">
@@ -10160,7 +10387,7 @@
         <v>776</v>
       </c>
       <c r="B421" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>472</v>
@@ -10169,10 +10396,10 @@
         <v>10000</v>
       </c>
       <c r="G421" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="H421" s="3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="422" spans="1:8" x14ac:dyDescent="0.25">
@@ -10180,7 +10407,7 @@
         <v>776</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>472</v>
@@ -10189,10 +10416,10 @@
         <v>10000</v>
       </c>
       <c r="G422" s="3" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="H422" s="3" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="423" spans="1:8" x14ac:dyDescent="0.25">
@@ -10200,7 +10427,7 @@
         <v>776</v>
       </c>
       <c r="B423" s="2" t="s">
-        <v>682</v>
+        <v>714</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>472</v>
@@ -10209,10 +10436,10 @@
         <v>10000</v>
       </c>
       <c r="G423" s="3" t="s">
-        <v>479</v>
+        <v>549</v>
       </c>
       <c r="H423" s="3" t="s">
-        <v>480</v>
+        <v>550</v>
       </c>
     </row>
     <row r="424" spans="1:8" x14ac:dyDescent="0.25">
@@ -10220,7 +10447,7 @@
         <v>776</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>472</v>
@@ -10229,10 +10456,10 @@
         <v>10000</v>
       </c>
       <c r="G424" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H424" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="425" spans="1:8" x14ac:dyDescent="0.25">
@@ -10240,7 +10467,7 @@
         <v>776</v>
       </c>
       <c r="B425" s="2" t="s">
-        <v>717</v>
+        <v>682</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>472</v>
@@ -10249,10 +10476,10 @@
         <v>10000</v>
       </c>
       <c r="G425" s="3" t="s">
-        <v>555</v>
+        <v>479</v>
       </c>
       <c r="H425" s="3" t="s">
-        <v>556</v>
+        <v>480</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.25">
@@ -10260,7 +10487,7 @@
         <v>776</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>472</v>
@@ -10269,10 +10496,10 @@
         <v>10000</v>
       </c>
       <c r="G426" s="3" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="H426" s="3" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.25">
@@ -10280,7 +10507,7 @@
         <v>776</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>472</v>
@@ -10289,10 +10516,10 @@
         <v>10000</v>
       </c>
       <c r="G427" s="3" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="H427" s="3" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="428" spans="1:8" x14ac:dyDescent="0.25">
@@ -10300,7 +10527,7 @@
         <v>776</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>472</v>
@@ -10309,10 +10536,10 @@
         <v>10000</v>
       </c>
       <c r="G428" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="H428" s="3" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="429" spans="1:8" x14ac:dyDescent="0.25">
@@ -10320,7 +10547,7 @@
         <v>776</v>
       </c>
       <c r="B429" s="2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>472</v>
@@ -10329,10 +10556,10 @@
         <v>10000</v>
       </c>
       <c r="G429" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H429" s="3" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="430" spans="1:8" x14ac:dyDescent="0.25">
@@ -10340,7 +10567,7 @@
         <v>776</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>472</v>
@@ -10349,10 +10576,10 @@
         <v>10000</v>
       </c>
       <c r="G430" s="3" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H430" s="3" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="431" spans="1:8" x14ac:dyDescent="0.25">
@@ -10360,7 +10587,7 @@
         <v>776</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>472</v>
@@ -10369,10 +10596,10 @@
         <v>10000</v>
       </c>
       <c r="G431" s="3" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="H431" s="3" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.25">
@@ -10380,7 +10607,7 @@
         <v>776</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>472</v>
@@ -10389,10 +10616,10 @@
         <v>10000</v>
       </c>
       <c r="G432" s="3" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="H432" s="3" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="433" spans="1:8" x14ac:dyDescent="0.25">
@@ -10400,7 +10627,7 @@
         <v>776</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>472</v>
@@ -10409,10 +10636,10 @@
         <v>10000</v>
       </c>
       <c r="G433" s="3" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="H433" s="3" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="434" spans="1:8" x14ac:dyDescent="0.25">
@@ -10420,7 +10647,7 @@
         <v>776</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>66</v>
+        <v>724</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>472</v>
@@ -10429,10 +10656,10 @@
         <v>10000</v>
       </c>
       <c r="G434" s="3" t="s">
-        <v>481</v>
+        <v>569</v>
       </c>
       <c r="H434" s="3" t="s">
-        <v>482</v>
+        <v>570</v>
       </c>
     </row>
     <row r="435" spans="1:8" x14ac:dyDescent="0.25">
@@ -10440,7 +10667,7 @@
         <v>776</v>
       </c>
       <c r="B435" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>472</v>
@@ -10449,10 +10676,10 @@
         <v>10000</v>
       </c>
       <c r="G435" s="3" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H435" s="3" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="436" spans="1:8" x14ac:dyDescent="0.25">
@@ -10460,7 +10687,7 @@
         <v>776</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>727</v>
+        <v>66</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>472</v>
@@ -10469,10 +10696,10 @@
         <v>10000</v>
       </c>
       <c r="G436" s="3" t="s">
-        <v>575</v>
+        <v>481</v>
       </c>
       <c r="H436" s="3" t="s">
-        <v>576</v>
+        <v>482</v>
       </c>
     </row>
     <row r="437" spans="1:8" x14ac:dyDescent="0.25">
@@ -10480,7 +10707,7 @@
         <v>776</v>
       </c>
       <c r="B437" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>472</v>
@@ -10489,10 +10716,10 @@
         <v>10000</v>
       </c>
       <c r="G437" s="3" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="H437" s="3" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="438" spans="1:8" x14ac:dyDescent="0.25">
@@ -10500,7 +10727,7 @@
         <v>776</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>472</v>
@@ -10509,10 +10736,10 @@
         <v>10000</v>
       </c>
       <c r="G438" s="3" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="H438" s="3" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="439" spans="1:8" x14ac:dyDescent="0.25">
@@ -10520,7 +10747,7 @@
         <v>776</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>472</v>
@@ -10529,10 +10756,10 @@
         <v>10000</v>
       </c>
       <c r="G439" s="3" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="H439" s="3" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="440" spans="1:8" x14ac:dyDescent="0.25">
@@ -10540,7 +10767,7 @@
         <v>776</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>472</v>
@@ -10549,10 +10776,10 @@
         <v>10000</v>
       </c>
       <c r="G440" s="3" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="H440" s="3" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="441" spans="1:8" x14ac:dyDescent="0.25">
@@ -10560,7 +10787,7 @@
         <v>776</v>
       </c>
       <c r="B441" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>472</v>
@@ -10569,10 +10796,10 @@
         <v>10000</v>
       </c>
       <c r="G441" s="3" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="H441" s="3" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="442" spans="1:8" x14ac:dyDescent="0.25">
@@ -10580,7 +10807,7 @@
         <v>776</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>472</v>
@@ -10589,10 +10816,10 @@
         <v>10000</v>
       </c>
       <c r="G442" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="H442" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="443" spans="1:8" x14ac:dyDescent="0.25">
@@ -10600,7 +10827,7 @@
         <v>776</v>
       </c>
       <c r="B443" s="2" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>472</v>
@@ -10609,10 +10836,10 @@
         <v>10000</v>
       </c>
       <c r="G443" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="H443" s="3" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="444" spans="1:8" x14ac:dyDescent="0.25">
@@ -10620,7 +10847,7 @@
         <v>776</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>472</v>
@@ -10629,10 +10856,10 @@
         <v>10000</v>
       </c>
       <c r="G444" s="3" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="H444" s="3" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="445" spans="1:8" x14ac:dyDescent="0.25">
@@ -10640,7 +10867,7 @@
         <v>776</v>
       </c>
       <c r="B445" s="2" t="s">
-        <v>683</v>
+        <v>734</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>472</v>
@@ -10649,10 +10876,10 @@
         <v>10000</v>
       </c>
       <c r="G445" s="3" t="s">
-        <v>483</v>
+        <v>589</v>
       </c>
       <c r="H445" s="3" t="s">
-        <v>484</v>
+        <v>590</v>
       </c>
     </row>
     <row r="446" spans="1:8" x14ac:dyDescent="0.25">
@@ -10660,7 +10887,7 @@
         <v>776</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>472</v>
@@ -10669,10 +10896,10 @@
         <v>10000</v>
       </c>
       <c r="G446" s="3" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H446" s="3" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="447" spans="1:8" x14ac:dyDescent="0.25">
@@ -10680,7 +10907,7 @@
         <v>776</v>
       </c>
       <c r="B447" s="2" t="s">
-        <v>737</v>
+        <v>683</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>472</v>
@@ -10689,10 +10916,10 @@
         <v>10000</v>
       </c>
       <c r="G447" s="3" t="s">
-        <v>595</v>
+        <v>483</v>
       </c>
       <c r="H447" s="3" t="s">
-        <v>596</v>
+        <v>484</v>
       </c>
     </row>
     <row r="448" spans="1:8" x14ac:dyDescent="0.25">
@@ -10700,7 +10927,7 @@
         <v>776</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>472</v>
@@ -10709,10 +10936,10 @@
         <v>10000</v>
       </c>
       <c r="G448" s="3" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="H448" s="3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="449" spans="1:8" x14ac:dyDescent="0.25">
@@ -10720,7 +10947,7 @@
         <v>776</v>
       </c>
       <c r="B449" s="2" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>472</v>
@@ -10729,10 +10956,10 @@
         <v>10000</v>
       </c>
       <c r="G449" s="3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H449" s="3" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="450" spans="1:8" x14ac:dyDescent="0.25">
@@ -10740,7 +10967,7 @@
         <v>776</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>472</v>
@@ -10749,10 +10976,10 @@
         <v>10000</v>
       </c>
       <c r="G450" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="H450" s="3" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="451" spans="1:8" x14ac:dyDescent="0.25">
@@ -10760,7 +10987,7 @@
         <v>776</v>
       </c>
       <c r="B451" s="2" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>472</v>
@@ -10769,10 +10996,10 @@
         <v>10000</v>
       </c>
       <c r="G451" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="H451" s="3" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="452" spans="1:8" x14ac:dyDescent="0.25">
@@ -10780,7 +11007,7 @@
         <v>776</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>472</v>
@@ -10789,10 +11016,10 @@
         <v>10000</v>
       </c>
       <c r="G452" s="3" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="H452" s="3" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="453" spans="1:8" x14ac:dyDescent="0.25">
@@ -10800,7 +11027,7 @@
         <v>776</v>
       </c>
       <c r="B453" s="2" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C453" s="2" t="s">
         <v>472</v>
@@ -10809,10 +11036,10 @@
         <v>10000</v>
       </c>
       <c r="G453" s="3" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="H453" s="3" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="454" spans="1:8" x14ac:dyDescent="0.25">
@@ -10820,7 +11047,7 @@
         <v>776</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>472</v>
@@ -10829,10 +11056,10 @@
         <v>10000</v>
       </c>
       <c r="G454" s="3" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="H454" s="3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="455" spans="1:8" x14ac:dyDescent="0.25">
@@ -10840,7 +11067,7 @@
         <v>776</v>
       </c>
       <c r="B455" s="2" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C455" s="2" t="s">
         <v>472</v>
@@ -10849,10 +11076,10 @@
         <v>10000</v>
       </c>
       <c r="G455" s="3" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="H455" s="3" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="456" spans="1:8" x14ac:dyDescent="0.25">
@@ -10860,7 +11087,7 @@
         <v>776</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>684</v>
+        <v>744</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>472</v>
@@ -10869,10 +11096,10 @@
         <v>10000</v>
       </c>
       <c r="G456" s="3" t="s">
-        <v>485</v>
+        <v>609</v>
       </c>
       <c r="H456" s="3" t="s">
-        <v>486</v>
+        <v>610</v>
       </c>
     </row>
     <row r="457" spans="1:8" x14ac:dyDescent="0.25">
@@ -10880,7 +11107,7 @@
         <v>776</v>
       </c>
       <c r="B457" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>472</v>
@@ -10889,10 +11116,10 @@
         <v>10000</v>
       </c>
       <c r="G457" s="3" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="H457" s="3" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="458" spans="1:8" x14ac:dyDescent="0.25">
@@ -10900,7 +11127,7 @@
         <v>776</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>747</v>
+        <v>684</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>472</v>
@@ -10909,10 +11136,10 @@
         <v>10000</v>
       </c>
       <c r="G458" s="3" t="s">
-        <v>615</v>
+        <v>485</v>
       </c>
       <c r="H458" s="3" t="s">
-        <v>614</v>
+        <v>486</v>
       </c>
     </row>
     <row r="459" spans="1:8" x14ac:dyDescent="0.25">
@@ -10920,7 +11147,7 @@
         <v>776</v>
       </c>
       <c r="B459" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>472</v>
@@ -10929,10 +11156,10 @@
         <v>10000</v>
       </c>
       <c r="G459" s="3" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="H459" s="3" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="460" spans="1:8" x14ac:dyDescent="0.25">
@@ -10940,7 +11167,7 @@
         <v>776</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>472</v>
@@ -10949,10 +11176,10 @@
         <v>10000</v>
       </c>
       <c r="G460" s="3" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="H460" s="3" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="461" spans="1:8" x14ac:dyDescent="0.25">
@@ -10960,7 +11187,7 @@
         <v>776</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C461" s="2" t="s">
         <v>472</v>
@@ -10969,10 +11196,10 @@
         <v>10000</v>
       </c>
       <c r="G461" s="3" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="H461" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.25">
@@ -10980,7 +11207,7 @@
         <v>776</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>472</v>
@@ -10989,10 +11216,10 @@
         <v>10000</v>
       </c>
       <c r="G462" s="3" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="H462" s="3" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.25">
@@ -11000,7 +11227,7 @@
         <v>776</v>
       </c>
       <c r="B463" s="2" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C463" s="2" t="s">
         <v>472</v>
@@ -11009,10 +11236,10 @@
         <v>10000</v>
       </c>
       <c r="G463" s="3" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="H463" s="3" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.25">
@@ -11020,7 +11247,7 @@
         <v>776</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C464" s="2" t="s">
         <v>472</v>
@@ -11029,10 +11256,10 @@
         <v>10000</v>
       </c>
       <c r="G464" s="3" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="H464" s="3" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.25">
@@ -11040,7 +11267,7 @@
         <v>776</v>
       </c>
       <c r="B465" s="2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>472</v>
@@ -11049,10 +11276,10 @@
         <v>10000</v>
       </c>
       <c r="G465" s="3" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="H465" s="3" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.25">
@@ -11060,7 +11287,7 @@
         <v>776</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>472</v>
@@ -11069,10 +11296,10 @@
         <v>10000</v>
       </c>
       <c r="G466" s="3" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="H466" s="3" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="467" spans="1:8" x14ac:dyDescent="0.25">
@@ -11080,7 +11307,7 @@
         <v>776</v>
       </c>
       <c r="B467" s="2" t="s">
-        <v>685</v>
+        <v>754</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>472</v>
@@ -11089,10 +11316,10 @@
         <v>10000</v>
       </c>
       <c r="G467" s="3" t="s">
-        <v>487</v>
+        <v>628</v>
       </c>
       <c r="H467" s="3" t="s">
-        <v>488</v>
+        <v>629</v>
       </c>
     </row>
     <row r="468" spans="1:8" x14ac:dyDescent="0.25">
@@ -11100,7 +11327,7 @@
         <v>776</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>472</v>
@@ -11109,10 +11336,10 @@
         <v>10000</v>
       </c>
       <c r="G468" s="3" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H468" s="3" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="469" spans="1:8" x14ac:dyDescent="0.25">
@@ -11120,7 +11347,7 @@
         <v>776</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>757</v>
+        <v>685</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>472</v>
@@ -11129,10 +11356,10 @@
         <v>10000</v>
       </c>
       <c r="G469" s="3" t="s">
-        <v>634</v>
+        <v>487</v>
       </c>
       <c r="H469" s="3" t="s">
-        <v>635</v>
+        <v>488</v>
       </c>
     </row>
     <row r="470" spans="1:8" x14ac:dyDescent="0.25">
@@ -11140,7 +11367,7 @@
         <v>776</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C470" s="2" t="s">
         <v>472</v>
@@ -11149,10 +11376,10 @@
         <v>10000</v>
       </c>
       <c r="G470" s="3" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="H470" s="3" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="471" spans="1:8" x14ac:dyDescent="0.25">
@@ -11160,7 +11387,7 @@
         <v>776</v>
       </c>
       <c r="B471" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C471" s="2" t="s">
         <v>472</v>
@@ -11169,10 +11396,10 @@
         <v>10000</v>
       </c>
       <c r="G471" s="3" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H471" s="3" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="472" spans="1:8" x14ac:dyDescent="0.25">
@@ -11180,7 +11407,7 @@
         <v>776</v>
       </c>
       <c r="B472" s="2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C472" s="2" t="s">
         <v>472</v>
@@ -11189,10 +11416,10 @@
         <v>10000</v>
       </c>
       <c r="G472" s="3" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="H472" s="3" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="473" spans="1:8" x14ac:dyDescent="0.25">
@@ -11200,7 +11427,7 @@
         <v>776</v>
       </c>
       <c r="B473" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C473" s="2" t="s">
         <v>472</v>
@@ -11209,10 +11436,10 @@
         <v>10000</v>
       </c>
       <c r="G473" s="3" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="H473" s="3" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="474" spans="1:8" x14ac:dyDescent="0.25">
@@ -11220,7 +11447,7 @@
         <v>776</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C474" s="2" t="s">
         <v>472</v>
@@ -11229,10 +11456,10 @@
         <v>10000</v>
       </c>
       <c r="G474" s="3" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="H474" s="3" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="475" spans="1:8" x14ac:dyDescent="0.25">
@@ -11240,7 +11467,7 @@
         <v>776</v>
       </c>
       <c r="B475" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C475" s="2" t="s">
         <v>472</v>
@@ -11249,10 +11476,10 @@
         <v>10000</v>
       </c>
       <c r="G475" s="3" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="H475" s="3" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="476" spans="1:8" x14ac:dyDescent="0.25">
@@ -11260,7 +11487,7 @@
         <v>776</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C476" s="2" t="s">
         <v>472</v>
@@ -11269,10 +11496,10 @@
         <v>10000</v>
       </c>
       <c r="G476" s="3" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="H476" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="477" spans="1:8" x14ac:dyDescent="0.25">
@@ -11280,7 +11507,7 @@
         <v>776</v>
       </c>
       <c r="B477" s="2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C477" s="2" t="s">
         <v>472</v>
@@ -11289,10 +11516,10 @@
         <v>10000</v>
       </c>
       <c r="G477" s="3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="H477" s="3" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="478" spans="1:8" x14ac:dyDescent="0.25">
@@ -11300,7 +11527,7 @@
         <v>776</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>686</v>
+        <v>764</v>
       </c>
       <c r="C478" s="2" t="s">
         <v>472</v>
@@ -11309,10 +11536,10 @@
         <v>10000</v>
       </c>
       <c r="G478" s="3" t="s">
-        <v>489</v>
+        <v>648</v>
       </c>
       <c r="H478" s="3" t="s">
-        <v>490</v>
+        <v>649</v>
       </c>
     </row>
     <row r="479" spans="1:8" x14ac:dyDescent="0.25">
@@ -11320,7 +11547,7 @@
         <v>776</v>
       </c>
       <c r="B479" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C479" s="2" t="s">
         <v>472</v>
@@ -11329,10 +11556,10 @@
         <v>10000</v>
       </c>
       <c r="G479" s="3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H479" s="3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="480" spans="1:8" x14ac:dyDescent="0.25">
@@ -11340,7 +11567,7 @@
         <v>776</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>767</v>
+        <v>686</v>
       </c>
       <c r="C480" s="2" t="s">
         <v>472</v>
@@ -11349,10 +11576,10 @@
         <v>10000</v>
       </c>
       <c r="G480" s="3" t="s">
-        <v>654</v>
+        <v>489</v>
       </c>
       <c r="H480" s="3" t="s">
-        <v>655</v>
+        <v>490</v>
       </c>
     </row>
     <row r="481" spans="1:8" x14ac:dyDescent="0.25">
@@ -11360,7 +11587,7 @@
         <v>776</v>
       </c>
       <c r="B481" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C481" s="2" t="s">
         <v>472</v>
@@ -11369,10 +11596,10 @@
         <v>10000</v>
       </c>
       <c r="G481" s="3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="H481" s="3" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="482" spans="1:8" x14ac:dyDescent="0.25">
@@ -11380,7 +11607,7 @@
         <v>776</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C482" s="2" t="s">
         <v>472</v>
@@ -11389,10 +11616,10 @@
         <v>10000</v>
       </c>
       <c r="G482" s="3" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="H482" s="3" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="483" spans="1:8" x14ac:dyDescent="0.25">
@@ -11400,7 +11627,7 @@
         <v>776</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C483" s="2" t="s">
         <v>472</v>
@@ -11409,10 +11636,10 @@
         <v>10000</v>
       </c>
       <c r="G483" s="3" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="H483" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="484" spans="1:8" x14ac:dyDescent="0.25">
@@ -11420,7 +11647,7 @@
         <v>776</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C484" s="2" t="s">
         <v>472</v>
@@ -11429,10 +11656,10 @@
         <v>10000</v>
       </c>
       <c r="G484" s="3" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="H484" s="3" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="485" spans="1:8" x14ac:dyDescent="0.25">
@@ -11440,7 +11667,7 @@
         <v>776</v>
       </c>
       <c r="B485" s="2" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C485" s="2" t="s">
         <v>472</v>
@@ -11449,10 +11676,10 @@
         <v>10000</v>
       </c>
       <c r="G485" s="3" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="H485" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="486" spans="1:8" x14ac:dyDescent="0.25">
@@ -11460,7 +11687,7 @@
         <v>776</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C486" s="2" t="s">
         <v>472</v>
@@ -11469,10 +11696,10 @@
         <v>10000</v>
       </c>
       <c r="G486" s="3" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="H486" s="3" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="487" spans="1:8" x14ac:dyDescent="0.25">
@@ -11480,7 +11707,7 @@
         <v>776</v>
       </c>
       <c r="B487" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C487" s="2" t="s">
         <v>472</v>
@@ -11489,10 +11716,10 @@
         <v>10000</v>
       </c>
       <c r="G487" s="3" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="H487" s="3" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="488" spans="1:8" x14ac:dyDescent="0.25">
@@ -11500,7 +11727,7 @@
         <v>776</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C488" s="2" t="s">
         <v>472</v>
@@ -11509,10 +11736,10 @@
         <v>10000</v>
       </c>
       <c r="G488" s="3" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="H488" s="3" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="489" spans="1:8" x14ac:dyDescent="0.25">
@@ -11520,7 +11747,7 @@
         <v>776</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>687</v>
+        <v>774</v>
       </c>
       <c r="C489" s="2" t="s">
         <v>472</v>
@@ -11529,38 +11756,50 @@
         <v>10000</v>
       </c>
       <c r="G489" s="3" t="s">
-        <v>491</v>
+        <v>668</v>
       </c>
       <c r="H489" s="3" t="s">
-        <v>492</v>
+        <v>669</v>
       </c>
     </row>
     <row r="490" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>799</v>
+        <v>776</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>451</v>
+        <v>775</v>
       </c>
       <c r="C490" s="2" t="s">
-        <v>262</v>
+        <v>472</v>
       </c>
       <c r="E490" s="1">
-        <v>25000</v>
+        <v>10000</v>
+      </c>
+      <c r="G490" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="H490" s="3" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="491" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>799</v>
+        <v>776</v>
       </c>
       <c r="B491" s="2" t="s">
-        <v>34</v>
+        <v>687</v>
       </c>
       <c r="C491" s="2" t="s">
-        <v>41</v>
+        <v>472</v>
       </c>
       <c r="E491" s="1">
-        <v>500000</v>
+        <v>10000</v>
+      </c>
+      <c r="G491" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="H491" s="3" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.25">
@@ -11568,13 +11807,13 @@
         <v>799</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>33</v>
+        <v>451</v>
       </c>
       <c r="C492" s="2" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="E492" s="1">
-        <v>50000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.25">
@@ -11582,13 +11821,13 @@
         <v>799</v>
       </c>
       <c r="B493" s="2" t="s">
-        <v>1068</v>
+        <v>34</v>
       </c>
       <c r="C493" s="2" t="s">
-        <v>1069</v>
+        <v>41</v>
       </c>
       <c r="E493" s="1">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.25">
@@ -11596,16 +11835,13 @@
         <v>799</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>1072</v>
+        <v>33</v>
       </c>
       <c r="C494" s="2" t="s">
-        <v>1074</v>
+        <v>40</v>
       </c>
       <c r="E494" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F494" s="1">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.25">
@@ -11613,16 +11849,13 @@
         <v>799</v>
       </c>
       <c r="B495" s="2" t="s">
-        <v>1073</v>
+        <v>1068</v>
       </c>
       <c r="C495" s="2" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
       <c r="E495" s="1">
-        <v>400</v>
-      </c>
-      <c r="F495" s="1">
-        <v>200</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="496" spans="1:8" x14ac:dyDescent="0.25">
@@ -11630,234 +11863,240 @@
         <v>799</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>35</v>
+        <v>1072</v>
       </c>
       <c r="C496" s="2" t="s">
-        <v>42</v>
+        <v>1074</v>
       </c>
       <c r="E496" s="1">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="497" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+      <c r="F496" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A497" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>38</v>
+        <v>1073</v>
       </c>
       <c r="C497" s="2" t="s">
-        <v>44</v>
+        <v>1075</v>
       </c>
       <c r="E497" s="1">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="498" spans="1:5" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="F497" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A498" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C498" s="2" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="E498" s="1">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A499" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C499" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="E499" s="1">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="500" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A500" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C500" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E500" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="501" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A501" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B501" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C501" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E501" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="502" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A502" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C502" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E502" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="503" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A503" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B503" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C503" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E503" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="504" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A504" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C504" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="E504" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="505" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B505" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C505" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E505" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C506" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E506" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="B507" s="2" t="s">
         <v>1070</v>
       </c>
-      <c r="C505" s="2" t="s">
+      <c r="C507" s="2" t="s">
         <v>1071</v>
       </c>
-      <c r="E505" s="1">
+      <c r="E507" s="1">
         <v>250000</v>
       </c>
     </row>
-    <row r="506" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A506" s="2" t="s">
-        <v>804</v>
-      </c>
-      <c r="B506" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="C506" s="2" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E506" s="1">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="507" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A507" s="2" t="s">
-        <v>804</v>
-      </c>
-      <c r="B507" s="2" t="s">
-        <v>805</v>
-      </c>
-      <c r="C507" s="2" t="s">
-        <v>1024</v>
-      </c>
-      <c r="E507" s="1">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="508" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A508" s="2" t="s">
         <v>804</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>806</v>
+        <v>822</v>
       </c>
       <c r="C508" s="2" t="s">
-        <v>1025</v>
+        <v>1041</v>
       </c>
       <c r="E508" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="509" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A509" s="2" t="s">
         <v>804</v>
       </c>
       <c r="B509" s="2" t="s">
-        <v>823</v>
+        <v>805</v>
       </c>
       <c r="C509" s="2" t="s">
-        <v>1042</v>
+        <v>1024</v>
       </c>
       <c r="E509" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="510" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
         <v>804</v>
       </c>
       <c r="B510" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C510" s="2" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="E510" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="511" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
         <v>804</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C511" s="2" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E511" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="512" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
         <v>804</v>
       </c>
       <c r="B512" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C512" s="2" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E512" s="1">
         <v>25000</v>
@@ -11868,10 +12107,10 @@
         <v>804</v>
       </c>
       <c r="B513" s="2" t="s">
-        <v>809</v>
+        <v>824</v>
       </c>
       <c r="C513" s="2" t="s">
-        <v>1028</v>
+        <v>1043</v>
       </c>
       <c r="E513" s="1">
         <v>25000</v>
@@ -11882,10 +12121,10 @@
         <v>804</v>
       </c>
       <c r="B514" s="2" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C514" s="2" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="E514" s="1">
         <v>25000</v>
@@ -11896,10 +12135,10 @@
         <v>804</v>
       </c>
       <c r="B515" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C515" s="2" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E515" s="1">
         <v>25000</v>
@@ -11910,10 +12149,10 @@
         <v>804</v>
       </c>
       <c r="B516" s="2" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C516" s="2" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E516" s="1">
         <v>25000</v>
@@ -11924,10 +12163,10 @@
         <v>804</v>
       </c>
       <c r="B517" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C517" s="2" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="E517" s="1">
         <v>25000</v>
@@ -11938,10 +12177,10 @@
         <v>804</v>
       </c>
       <c r="B518" s="2" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C518" s="2" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="E518" s="1">
         <v>25000</v>
@@ -11952,10 +12191,10 @@
         <v>804</v>
       </c>
       <c r="B519" s="2" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C519" s="2" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E519" s="1">
         <v>25000</v>
@@ -11966,10 +12205,10 @@
         <v>804</v>
       </c>
       <c r="B520" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C520" s="2" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="E520" s="1">
         <v>25000</v>
@@ -11980,10 +12219,10 @@
         <v>804</v>
       </c>
       <c r="B521" s="2" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="C521" s="2" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="E521" s="1">
         <v>25000</v>
@@ -11994,10 +12233,10 @@
         <v>804</v>
       </c>
       <c r="B522" s="2" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c r="C522" s="2" t="s">
-        <v>1045</v>
+        <v>1035</v>
       </c>
       <c r="E522" s="1">
         <v>25000</v>
@@ -12008,10 +12247,10 @@
         <v>804</v>
       </c>
       <c r="B523" s="2" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C523" s="2" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E523" s="1">
         <v>25000</v>
@@ -12022,10 +12261,10 @@
         <v>804</v>
       </c>
       <c r="B524" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="C524" s="2" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="E524" s="1">
         <v>25000</v>
@@ -12036,10 +12275,10 @@
         <v>804</v>
       </c>
       <c r="B525" s="2" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C525" s="2" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="E525" s="1">
         <v>25000</v>
@@ -12050,10 +12289,10 @@
         <v>804</v>
       </c>
       <c r="B526" s="2" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C526" s="2" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="E526" s="1">
         <v>25000</v>
@@ -12064,10 +12303,10 @@
         <v>804</v>
       </c>
       <c r="B527" s="2" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C527" s="2" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E527" s="1">
         <v>25000</v>
@@ -12078,10 +12317,10 @@
         <v>804</v>
       </c>
       <c r="B528" s="2" t="s">
-        <v>817</v>
+        <v>830</v>
       </c>
       <c r="C528" s="2" t="s">
-        <v>1036</v>
+        <v>1049</v>
       </c>
       <c r="E528" s="1">
         <v>25000</v>
@@ -12092,10 +12331,10 @@
         <v>804</v>
       </c>
       <c r="B529" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C529" s="2" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E529" s="1">
         <v>25000</v>
@@ -12106,10 +12345,10 @@
         <v>804</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>833</v>
+        <v>817</v>
       </c>
       <c r="C530" s="2" t="s">
-        <v>1052</v>
+        <v>1036</v>
       </c>
       <c r="E530" s="1">
         <v>25000</v>
@@ -12120,10 +12359,10 @@
         <v>804</v>
       </c>
       <c r="B531" s="2" t="s">
-        <v>818</v>
+        <v>832</v>
       </c>
       <c r="C531" s="2" t="s">
-        <v>1037</v>
+        <v>1051</v>
       </c>
       <c r="E531" s="1">
         <v>25000</v>
@@ -12134,10 +12373,10 @@
         <v>804</v>
       </c>
       <c r="B532" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C532" s="2" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E532" s="1">
         <v>25000</v>
@@ -12148,10 +12387,10 @@
         <v>804</v>
       </c>
       <c r="B533" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C533" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E533" s="1">
         <v>25000</v>
@@ -12162,10 +12401,10 @@
         <v>804</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C534" s="2" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E534" s="1">
         <v>25000</v>
@@ -12176,10 +12415,10 @@
         <v>804</v>
       </c>
       <c r="B535" s="2" t="s">
-        <v>836</v>
+        <v>819</v>
       </c>
       <c r="C535" s="2" t="s">
-        <v>1055</v>
+        <v>1038</v>
       </c>
       <c r="E535" s="1">
         <v>25000</v>
@@ -12190,10 +12429,10 @@
         <v>804</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>820</v>
+        <v>835</v>
       </c>
       <c r="C536" s="2" t="s">
-        <v>1039</v>
+        <v>1054</v>
       </c>
       <c r="E536" s="1">
         <v>25000</v>
@@ -12204,10 +12443,10 @@
         <v>804</v>
       </c>
       <c r="B537" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C537" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E537" s="1">
         <v>25000</v>
@@ -12218,10 +12457,10 @@
         <v>804</v>
       </c>
       <c r="B538" s="2" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="C538" s="2" t="s">
-        <v>1057</v>
+        <v>1039</v>
       </c>
       <c r="E538" s="1">
         <v>25000</v>
@@ -12232,21 +12471,49 @@
         <v>804</v>
       </c>
       <c r="B539" s="2" t="s">
-        <v>821</v>
+        <v>837</v>
       </c>
       <c r="C539" s="2" t="s">
-        <v>1040</v>
+        <v>1056</v>
       </c>
       <c r="E539" s="1">
         <v>25000</v>
       </c>
     </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A540" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B540" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="C540" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E540" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A541" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="C541" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E541" s="1">
+        <v>25000</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H539">
-    <sortCondition ref="A2:A539"/>
-    <sortCondition ref="C2:C539"/>
-    <sortCondition ref="D2:D539"/>
-    <sortCondition ref="H2:H539"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H541">
+    <sortCondition ref="A2:A541"/>
+    <sortCondition ref="C2:C541"/>
+    <sortCondition ref="D2:D541"/>
+    <sortCondition ref="H2:H541"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>